<commit_message>
Thai Quoc Toan upload fix error student management - admin
</commit_message>
<xml_diff>
--- a/OJTManagementSystem/src/main/webapp/excels/evaluarionStudent.xlsx
+++ b/OJTManagementSystem/src/main/webapp/excels/evaluarionStudent.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Stdudent Code</t>
   </si>
@@ -35,19 +35,16 @@
     <t>Status</t>
   </si>
   <si>
-    <t>SE151272</t>
+    <t>SE151252</t>
   </si>
   <si>
     <t>Kỹ thuật phần mềm</t>
   </si>
   <si>
-    <t>AMERICAN STUDY</t>
+    <t>BAP GROUP</t>
   </si>
   <si>
-    <t>Ngôn ngữ anh</t>
-  </si>
-  <si>
-    <t>Tốt, Giỏi</t>
+    <t>Nhiệt huyết trong công việc.</t>
   </si>
   <si>
     <t>Passed</t>
@@ -156,16 +153,16 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Thai Quoc Toan Upload fix functions
</commit_message>
<xml_diff>
--- a/OJTManagementSystem/src/main/webapp/excels/evaluarionStudent.xlsx
+++ b/OJTManagementSystem/src/main/webapp/excels/evaluarionStudent.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Stdudent Code</t>
   </si>
@@ -35,28 +35,40 @@
     <t>Status</t>
   </si>
   <si>
+    <t>SE151252</t>
+  </si>
+  <si>
+    <t>Kỹ thuật phần mềm</t>
+  </si>
+  <si>
+    <t>BAP GROUP</t>
+  </si>
+  <si>
+    <t>Nhiệt huyết trong công việc.</t>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>SE151272</t>
+  </si>
+  <si>
+    <t>NASHTECH</t>
+  </si>
+  <si>
+    <t>Hoàn thành tốt.</t>
+  </si>
+  <si>
     <t>SE151262</t>
   </si>
   <si>
-    <t>Kỹ thuật phần mềm</t>
-  </si>
-  <si>
-    <t>AMERICAN STUDY</t>
-  </si>
-  <si>
-    <t>Ngôn ngữ anh</t>
-  </si>
-  <si>
-    <t>Không hoàn thành</t>
-  </si>
-  <si>
-    <t>Not Pass</t>
-  </si>
-  <si>
-    <t>SE150003</t>
-  </si>
-  <si>
-    <t>ngu</t>
+    <t>MANULIFE</t>
+  </si>
+  <si>
+    <t>Kinh doanh quốc tế</t>
+  </si>
+  <si>
+    <t>Thực hiện tốt nhiệm vụ giao.</t>
   </si>
 </sst>
 </file>
@@ -112,9 +124,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
@@ -123,7 +136,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -163,39 +176,62 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3" t="n">
-        <v>2.5</v>
+        <v>6.0</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Thai Quoc Toan fix bugs
</commit_message>
<xml_diff>
--- a/OJTManagementSystem/src/main/webapp/excels/evaluarionStudent.xlsx
+++ b/OJTManagementSystem/src/main/webapp/excels/evaluarionStudent.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Stdudent Code</t>
   </si>
@@ -48,15 +48,6 @@
   </si>
   <si>
     <t>Passed</t>
-  </si>
-  <si>
-    <t>SE151272</t>
-  </si>
-  <si>
-    <t>Go2Joy Vietnam JSC</t>
-  </si>
-  <si>
-    <t>Tinh thần học tập cao, hoàn thành tốt các nhiệm vụ được giao, năng động, tích cực.</t>
   </si>
 </sst>
 </file>
@@ -112,10 +103,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="true" applyFill="true" applyBorder="true"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
 </styleSheet>
@@ -123,7 +113,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -175,29 +165,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>